<commit_message>
i need a gitignor :(
</commit_message>
<xml_diff>
--- a/files/output.xlsx
+++ b/files/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="page-1-table-1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,89 +422,80 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2025.03.18. (KEDD)</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr"/>
+      <c r="J1" t="inlineStr"/>
+      <c r="K1" t="inlineStr"/>
+      <c r="L1" t="inlineStr"/>
+      <c r="M1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Helyettesített
+pedagógus neve</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Típus</t>
+          <t>supíT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hanyadik óra</t>
+          <t>aró
+kidaynáH</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Osztály</t>
+          <t>ylátzsO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tantárgy
-megnevezése</t>
+          <t>Tantárgy megnevezése</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Helyettesítést
-végző
-pedagógus
-neve</t>
+          <t>Helyettesítést végző
+pedagógus neve</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Óracsere esetén 
-hová/honnan</t>
+          <t>Óracsere esetén hová került</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
+          <t>Óracsere esetén honnan került ide</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>Teremcsere esetén</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -527,7 +506,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ténylegesen</t>
+          <t>Ténylegesen</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -543,219 +522,202 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>dáum</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>óra</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>honnan</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>hová</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Őzéné G. J.</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>2.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.a-hal</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>9.ny-ker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>gépírás</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ang</t>
+          <t>matematika</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Békei J.</t>
+          <t>Rozsiszkyné A. Á. O.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>SZT2</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Korom R.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>9.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.b</t>
+          <t>11.c-inf</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Tört</t>
+          <t>--</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>web_prog</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025.03.19.</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>SZT1</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>-
-cs</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Márton D.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>7.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.b</t>
+          <t>13.b</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Of</t>
+          <t>fogyasztóvédelem</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Fiz</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Janó É.</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025.03.17.</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>3.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>15.</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>cs</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>10.b</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Fiz</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Tört</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Kiss G.</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tartóczky E.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>35.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.b-kezd</t>
+          <t>9.c-kezdő</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ang</t>
+          <t>angol</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>--</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -763,64 +725,43 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>-
-cs</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>2.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10.c-kezd</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>11.c-kezdő</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>angol</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ném</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Kónya M.</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>10.18.</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>K1</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>3.</t>
@@ -828,17 +769,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11.a</t>
+          <t>2/14.b</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Tört</t>
+          <t>munk_id_nyelv</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>feladat</t>
+          <t>ül</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -846,346 +787,315 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>4.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11.c</t>
+          <t>9.a-haladó</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Mat/Kisg</t>
+          <t>angol</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>ül</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Kissné Á. M. (H)</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>tanári_ebédlő</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>cs</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kormányos A.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
         <is>
           <t>2.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>11.c-gazd</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Titk</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Üzl</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Kendik R.</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>10. 20.</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>-
-cs</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11.c-gazd</t>
+          <t>12.c-kezdő</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Tört</t>
+          <t>IKT_proj_munk_II</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Kisg</t>
+          <t>IKT_proj_munk_II</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Faragóné Z. A.</t>
+          <t>Bálint R.</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>32.</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>34.</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>-
-cs</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6.</t>
+          <t>4.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11.c-inf</t>
+          <t>2/14.b</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Tört</t>
+          <t>IKT_proj_munk_II</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Mat</t>
+          <t>Backend</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Murár Z.</t>
+          <t>Gyuris Cs.</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>14.</t>
-        </is>
-      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>34.</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>5.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12.c</t>
+          <t>2/14.b</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Tört</t>
+          <t>IKT_proj_munk_II</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>film</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>IKT_proj_munk_II</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Berczik A.</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2025.03.21.</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>34.</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>-
-cs</t>
-        </is>
-      </c>
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>6.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12.c-kezd</t>
+          <t>12.c-haladó</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Ném</t>
+          <t>web_prog</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Ang</t>
+          <t>web_prog</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Kucsó K.</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>10. 19.</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
+          <t>Zsivola M.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>taniroda</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
         <is>
           <t>7.</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>K3</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>9.a-kezd</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>12.b-haladó</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>IKT_proj_munk_II</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Mat</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Kiss A.</t>
-        </is>
-      </c>
+          <t>ül</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>nyelvi labor</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.</t>
+          <t>8.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>9.a-kezd</t>
+          <t>12.b-haladó</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Ang</t>
+          <t>web_prog</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ül</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1193,76 +1103,156 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>SZT1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>9.b</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Tört</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Gyuris Cs.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.</t>
+          <t>1.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>9.c</t>
+          <t>2/14.b</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Irod</t>
+          <t>Backend</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>--</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bálint R.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12.c-kezdő</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>IKT_proj_munk_II</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Zsivola M.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>12.c-haladó</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>web_prog</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025.03.18.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>